<commit_message>
Discovered when screen/color/UDGs are stored
</commit_message>
<xml_diff>
--- a/memory_map.xlsx
+++ b/memory_map.xlsx
@@ -7,16 +7,15 @@
     <workbookView xWindow="384" yWindow="72" windowWidth="29988" windowHeight="13800"/>
   </bookViews>
   <sheets>
-    <sheet name="VIC-20 8K+ EXPANSION" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="JETPAC VIC-20 8K+ Expansion" sheetId="6" r:id="rId1"/>
+    <sheet name="Default VIC-20 8K+ Expansion " sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="35">
   <si>
     <t>A</t>
   </si>
@@ -135,6 +134,12 @@
       </rPr>
       <t xml:space="preserve"> MAP</t>
     </r>
+  </si>
+  <si>
+    <t>USER DEFINED CHARACTER SET RAM</t>
+  </si>
+  <si>
+    <t>Not Used</t>
   </si>
 </sst>
 </file>
@@ -382,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -411,7 +416,13 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -490,6 +501,33 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -796,22 +834,22 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:R9"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="34"/>
+    <col min="1" max="1" width="8.88671875" style="36"/>
     <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="18" width="6.5546875" customWidth="1"/>
     <col min="19" max="31" width="3.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="36"/>
+      <c r="B1" s="38"/>
       <c r="C1" s="1">
         <v>0</v>
       </c>
@@ -862,7 +900,7 @@
       </c>
     </row>
     <row r="2" spans="1:18" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A2" s="35">
+      <c r="A2" s="37">
         <f>HEX2DEC(B2)</f>
         <v>61440</v>
       </c>
@@ -889,7 +927,7 @@
       <c r="R2" s="7"/>
     </row>
     <row r="3" spans="1:18" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A3" s="35">
+      <c r="A3" s="37">
         <f t="shared" ref="A3:A17" si="0">HEX2DEC(B3)</f>
         <v>57344</v>
       </c>
@@ -914,7 +952,7 @@
       <c r="R3" s="7"/>
     </row>
     <row r="4" spans="1:18" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A4" s="35">
+      <c r="A4" s="37">
         <f t="shared" si="0"/>
         <v>53248</v>
       </c>
@@ -941,7 +979,7 @@
       <c r="R4" s="7"/>
     </row>
     <row r="5" spans="1:18" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A5" s="35">
+      <c r="A5" s="37">
         <f t="shared" si="0"/>
         <v>49152</v>
       </c>
@@ -966,7 +1004,600 @@
       <c r="R5" s="7"/>
     </row>
     <row r="6" spans="1:18" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A6" s="35">
+      <c r="A6" s="37">
+        <f t="shared" si="0"/>
+        <v>45056</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="39"/>
+      <c r="M6" s="39"/>
+      <c r="N6" s="39"/>
+      <c r="O6" s="39"/>
+      <c r="P6" s="39"/>
+      <c r="Q6" s="39"/>
+      <c r="R6" s="39"/>
+    </row>
+    <row r="7" spans="1:18" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A7" s="37">
+        <f t="shared" si="0"/>
+        <v>40960</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="39"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="40"/>
+      <c r="O7" s="40"/>
+      <c r="P7" s="40"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="40"/>
+    </row>
+    <row r="8" spans="1:18" ht="31.2" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A8" s="37">
+        <f t="shared" si="0"/>
+        <v>36864</v>
+      </c>
+      <c r="B8" s="2">
+        <v>9000</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="31">
+        <f>HEX2DEC(B8) + (HEX2DEC(D18)*256)</f>
+        <v>37120</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="27"/>
+      <c r="G8" s="32">
+        <f>HEX2DEC(B8) + (HEX2DEC(G18)*256)</f>
+        <v>37888</v>
+      </c>
+      <c r="H8" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" s="29">
+        <f>HEX2DEC(B8) + (HEX2DEC(I18)*256)</f>
+        <v>38400</v>
+      </c>
+      <c r="J8" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="44">
+        <f>HEX2DEC(B8) + (HEX2DEC(K18)*256)</f>
+        <v>38912</v>
+      </c>
+      <c r="L8" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="45"/>
+      <c r="N8" s="45"/>
+      <c r="O8" s="46">
+        <f>HEX2DEC(B8) + (HEX2DEC(O18)*256)</f>
+        <v>39936</v>
+      </c>
+      <c r="P8" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q8" s="45"/>
+      <c r="R8" s="47"/>
+    </row>
+    <row r="9" spans="1:18" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A9" s="37">
+        <f t="shared" si="0"/>
+        <v>32768</v>
+      </c>
+      <c r="B9" s="2">
+        <v>8000</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="24"/>
+      <c r="R9" s="24"/>
+    </row>
+    <row r="10" spans="1:18" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A10" s="37">
+        <f t="shared" si="0"/>
+        <v>28672</v>
+      </c>
+      <c r="B10" s="2">
+        <v>7000</v>
+      </c>
+      <c r="C10" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="39"/>
+      <c r="O10" s="39"/>
+      <c r="P10" s="39"/>
+      <c r="Q10" s="39"/>
+      <c r="R10" s="39"/>
+    </row>
+    <row r="11" spans="1:18" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A11" s="37">
+        <f t="shared" si="0"/>
+        <v>24576</v>
+      </c>
+      <c r="B11" s="2">
+        <v>6000</v>
+      </c>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="39"/>
+      <c r="N11" s="39"/>
+      <c r="O11" s="39"/>
+      <c r="P11" s="39"/>
+      <c r="Q11" s="39"/>
+      <c r="R11" s="39"/>
+    </row>
+    <row r="12" spans="1:18" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A12" s="37">
+        <f t="shared" si="0"/>
+        <v>20480</v>
+      </c>
+      <c r="B12" s="2">
+        <v>5000</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="39"/>
+      <c r="L12" s="39"/>
+      <c r="M12" s="39"/>
+      <c r="N12" s="39"/>
+      <c r="O12" s="39"/>
+      <c r="P12" s="39"/>
+      <c r="Q12" s="39"/>
+      <c r="R12" s="39"/>
+    </row>
+    <row r="13" spans="1:18" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A13" s="37">
+        <f t="shared" si="0"/>
+        <v>16384</v>
+      </c>
+      <c r="B13" s="2">
+        <v>4000</v>
+      </c>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="39"/>
+      <c r="L13" s="39"/>
+      <c r="M13" s="39"/>
+      <c r="N13" s="39"/>
+      <c r="O13" s="39"/>
+      <c r="P13" s="39"/>
+      <c r="Q13" s="39"/>
+      <c r="R13" s="39"/>
+    </row>
+    <row r="14" spans="1:18" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A14" s="37">
+        <f t="shared" si="0"/>
+        <v>12288</v>
+      </c>
+      <c r="B14" s="2">
+        <v>3000</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+    </row>
+    <row r="15" spans="1:18" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A15" s="37">
+        <f t="shared" si="0"/>
+        <v>8192</v>
+      </c>
+      <c r="B15" s="2">
+        <v>2000</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+    </row>
+    <row r="16" spans="1:18" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A16" s="37">
+        <f t="shared" si="0"/>
+        <v>4096</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1000</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="12"/>
+    </row>
+    <row r="17" spans="1:18" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A17" s="37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="13"/>
+      <c r="G17" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
+      <c r="K17" s="42"/>
+      <c r="L17" s="42"/>
+      <c r="M17" s="42"/>
+      <c r="N17" s="42"/>
+      <c r="O17" s="42"/>
+      <c r="P17" s="42"/>
+      <c r="Q17" s="42"/>
+      <c r="R17" s="43"/>
+    </row>
+    <row r="18" spans="1:18" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <v>2</v>
+      </c>
+      <c r="F18" s="1">
+        <v>3</v>
+      </c>
+      <c r="G18" s="1">
+        <v>4</v>
+      </c>
+      <c r="H18" s="1">
+        <v>5</v>
+      </c>
+      <c r="I18" s="1">
+        <v>6</v>
+      </c>
+      <c r="J18" s="1">
+        <v>7</v>
+      </c>
+      <c r="K18" s="1">
+        <v>8</v>
+      </c>
+      <c r="L18" s="1">
+        <v>9</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="C16:R16"/>
+    <mergeCell ref="G17:R17"/>
+    <mergeCell ref="C9:R9"/>
+    <mergeCell ref="C10:R11"/>
+    <mergeCell ref="C12:R13"/>
+    <mergeCell ref="C14:R15"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C2:R3"/>
+    <mergeCell ref="C4:R5"/>
+    <mergeCell ref="C6:R7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="P8:R8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R18"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="36"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="18" width="6.5546875" customWidth="1"/>
+    <col min="19" max="31" width="3.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A1" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="1">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1">
+        <v>8</v>
+      </c>
+      <c r="L1" s="1">
+        <v>9</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A2" s="37">
+        <f>HEX2DEC(B2)</f>
+        <v>61440</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+    </row>
+    <row r="3" spans="1:18" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A3" s="37">
+        <f t="shared" ref="A3:A17" si="0">HEX2DEC(B3)</f>
+        <v>57344</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+    </row>
+    <row r="4" spans="1:18" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A4" s="37">
+        <f t="shared" si="0"/>
+        <v>53248</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+    </row>
+    <row r="5" spans="1:18" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A5" s="37">
+        <f t="shared" si="0"/>
+        <v>49152</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+    </row>
+    <row r="6" spans="1:18" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A6" s="37">
         <f t="shared" si="0"/>
         <v>45056</v>
       </c>
@@ -993,7 +1624,7 @@
       <c r="R6" s="6"/>
     </row>
     <row r="7" spans="1:18" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A7" s="35">
+      <c r="A7" s="37">
         <f t="shared" si="0"/>
         <v>40960</v>
       </c>
@@ -1001,76 +1632,76 @@
         <v>10</v>
       </c>
       <c r="C7" s="6"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="21"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
     </row>
     <row r="8" spans="1:18" ht="31.2" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A8" s="35">
+      <c r="A8" s="37">
         <f t="shared" si="0"/>
         <v>36864</v>
       </c>
       <c r="B8" s="2">
         <v>9000</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="29">
+      <c r="D8" s="31">
         <f>HEX2DEC(B8) + (HEX2DEC(D18)*256)</f>
         <v>37120</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="25"/>
-      <c r="G8" s="27">
+      <c r="F8" s="27"/>
+      <c r="G8" s="29">
         <f>HEX2DEC(B8) + (HEX2DEC(G18)*256)</f>
         <v>37888</v>
       </c>
-      <c r="H8" s="31" t="s">
+      <c r="H8" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="I8" s="30">
+      <c r="I8" s="32">
         <f>HEX2DEC(B8) + (HEX2DEC(I18)*256)</f>
         <v>38400</v>
       </c>
-      <c r="J8" s="32" t="s">
+      <c r="J8" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="K8" s="33">
+      <c r="K8" s="35">
         <f>HEX2DEC(B8) + (HEX2DEC(K18)*256)</f>
         <v>38912</v>
       </c>
-      <c r="L8" s="23" t="s">
+      <c r="L8" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="29">
+      <c r="M8" s="25"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="31">
         <f>HEX2DEC(B8) + (HEX2DEC(O18)*256)</f>
         <v>39936</v>
       </c>
-      <c r="P8" s="23" t="s">
+      <c r="P8" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="Q8" s="23"/>
-      <c r="R8" s="24"/>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="26"/>
     </row>
     <row r="9" spans="1:18" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A9" s="35">
+      <c r="A9" s="37">
         <f t="shared" si="0"/>
         <v>32768</v>
       </c>
@@ -1080,24 +1711,24 @@
       <c r="C9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22"/>
-      <c r="O9" s="22"/>
-      <c r="P9" s="22"/>
-      <c r="Q9" s="22"/>
-      <c r="R9" s="22"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="24"/>
+      <c r="R9" s="24"/>
     </row>
     <row r="10" spans="1:18" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A10" s="35">
+      <c r="A10" s="37">
         <f t="shared" si="0"/>
         <v>28672</v>
       </c>
@@ -1124,7 +1755,7 @@
       <c r="R10" s="8"/>
     </row>
     <row r="11" spans="1:18" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A11" s="35">
+      <c r="A11" s="37">
         <f t="shared" si="0"/>
         <v>24576</v>
       </c>
@@ -1149,7 +1780,7 @@
       <c r="R11" s="8"/>
     </row>
     <row r="12" spans="1:18" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A12" s="35">
+      <c r="A12" s="37">
         <f t="shared" si="0"/>
         <v>20480</v>
       </c>
@@ -1176,7 +1807,7 @@
       <c r="R12" s="8"/>
     </row>
     <row r="13" spans="1:18" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A13" s="35">
+      <c r="A13" s="37">
         <f t="shared" si="0"/>
         <v>16384</v>
       </c>
@@ -1201,7 +1832,7 @@
       <c r="R13" s="8"/>
     </row>
     <row r="14" spans="1:18" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A14" s="35">
+      <c r="A14" s="37">
         <f t="shared" si="0"/>
         <v>12288</v>
       </c>
@@ -1228,7 +1859,7 @@
       <c r="R14" s="8"/>
     </row>
     <row r="15" spans="1:18" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A15" s="35">
+      <c r="A15" s="37">
         <f t="shared" si="0"/>
         <v>8192</v>
       </c>
@@ -1237,23 +1868,23 @@
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="12"/>
-      <c r="Q15" s="12"/>
-      <c r="R15" s="12"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
     </row>
     <row r="16" spans="1:18" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A16" s="35">
+      <c r="A16" s="37">
         <f t="shared" si="0"/>
         <v>4096</v>
       </c>
@@ -1263,29 +1894,29 @@
       <c r="C16" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="14">
+      <c r="D16" s="13"/>
+      <c r="E16" s="16">
         <f>HEX2DEC(B16) + (HEX2DEC(E18)*256)</f>
         <v>4608</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18"/>
-      <c r="O16" s="18"/>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="18"/>
-      <c r="R16" s="19"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="20"/>
+      <c r="O16" s="20"/>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="20"/>
+      <c r="R16" s="21"/>
     </row>
     <row r="17" spans="1:18" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A17" s="35">
+      <c r="A17" s="37">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1298,27 +1929,27 @@
       <c r="D17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F17" s="17"/>
-      <c r="G17" s="20">
+      <c r="F17" s="19"/>
+      <c r="G17" s="22">
         <f>HEX2DEC(B17) + (HEX2DEC(G18)*256)</f>
         <v>1024</v>
       </c>
-      <c r="H17" s="15" t="s">
+      <c r="H17" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="16"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="18"/>
     </row>
     <row r="18" spans="1:18" ht="31.2" x14ac:dyDescent="0.6">
       <c r="C18" s="1">
@@ -1394,28 +2025,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Identified Num_Lives at a via MAME debug save n_lives.bin,0000,1fff compares
</commit_message>
<xml_diff>
--- a/memory_map.xlsx
+++ b/memory_map.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="JETPAC VIC-20 8K+ Expansion" sheetId="6" r:id="rId1"/>
     <sheet name="Default VIC-20 8K+ Expansion " sheetId="1" r:id="rId2"/>
+    <sheet name="Memory Trace" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="79">
   <si>
     <t>A</t>
   </si>
@@ -141,13 +142,153 @@
   <si>
     <t>Not Used</t>
   </si>
+  <si>
+    <t>201d</t>
+  </si>
+  <si>
+    <t>20b2</t>
+  </si>
+  <si>
+    <t>20bc</t>
+  </si>
+  <si>
+    <t>20c6</t>
+  </si>
+  <si>
+    <t>20ad</t>
+  </si>
+  <si>
+    <t>20b7</t>
+  </si>
+  <si>
+    <t>20c1</t>
+  </si>
+  <si>
+    <t>20cb</t>
+  </si>
+  <si>
+    <t>20d0</t>
+  </si>
+  <si>
+    <t>20e2</t>
+  </si>
+  <si>
+    <t>2416</t>
+  </si>
+  <si>
+    <t>244f</t>
+  </si>
+  <si>
+    <t>24a4</t>
+  </si>
+  <si>
+    <t>24cc</t>
+  </si>
+  <si>
+    <t>24d4</t>
+  </si>
+  <si>
+    <t>24d9</t>
+  </si>
+  <si>
+    <t>24ed</t>
+  </si>
+  <si>
+    <t>251e</t>
+  </si>
+  <si>
+    <t>259e</t>
+  </si>
+  <si>
+    <t>25cd</t>
+  </si>
+  <si>
+    <t>25d0</t>
+  </si>
+  <si>
+    <t>265e</t>
+  </si>
+  <si>
+    <t>2668</t>
+  </si>
+  <si>
+    <t>275b</t>
+  </si>
+  <si>
+    <t>2763</t>
+  </si>
+  <si>
+    <t>276f</t>
+  </si>
+  <si>
+    <t>2779</t>
+  </si>
+  <si>
+    <t>34a6</t>
+  </si>
+  <si>
+    <t>34c3</t>
+  </si>
+  <si>
+    <t>34c7</t>
+  </si>
+  <si>
+    <t>3511</t>
+  </si>
+  <si>
+    <t>3520</t>
+  </si>
+  <si>
+    <t>3544</t>
+  </si>
+  <si>
+    <t>355c</t>
+  </si>
+  <si>
+    <t>357b</t>
+  </si>
+  <si>
+    <t>35d6</t>
+  </si>
+  <si>
+    <t>Block Len</t>
+  </si>
+  <si>
+    <t>Block Start</t>
+  </si>
+  <si>
+    <t>Block End</t>
+  </si>
+  <si>
+    <t>Gap</t>
+  </si>
+  <si>
+    <t>Game Select only</t>
+  </si>
+  <si>
+    <t>Start Up + Game Select</t>
+  </si>
+  <si>
+    <t>208f</t>
+  </si>
+  <si>
+    <t>34cc</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -198,7 +339,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -262,6 +403,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -387,108 +534,108 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -500,35 +647,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -833,7 +1000,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -2025,4 +2192,554 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.77734375" style="48" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="48"/>
+    <col min="3" max="3" width="8.77734375" style="50" bestFit="1" customWidth="1"/>
+    <col min="4" max="22" width="8.88671875" style="49"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="52" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="52"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54"/>
+      <c r="V1" s="54"/>
+    </row>
+    <row r="2" spans="1:22" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="52" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="52" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="54" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="54"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="54"/>
+      <c r="S2" s="54"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="54"/>
+      <c r="V2" s="54"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A3" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="51">
+        <f>HEX2DEC(B3)-HEX2DEC(A3)</f>
+        <v>144</v>
+      </c>
+      <c r="F3" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="G3" s="50" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="57">
+        <f>HEX2DEC(G3)-HEX2DEC(F3)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A4" s="48" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="51">
+        <f t="shared" ref="C4:C21" si="0">HEX2DEC(B4)-HEX2DEC(A4)</f>
+        <v>5</v>
+      </c>
+      <c r="D4" s="48">
+        <f>HEX2DEC(A4)-HEX2DEC(B3)</f>
+        <v>5</v>
+      </c>
+      <c r="F4" s="51" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="51">
+        <f t="shared" ref="H4:H21" si="1">HEX2DEC(G4)-HEX2DEC(F4)</f>
+        <v>5</v>
+      </c>
+      <c r="I4" s="48"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A5" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="51">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D5" s="48">
+        <f t="shared" ref="D5:D21" si="2">HEX2DEC(A5)-HEX2DEC(B4)</f>
+        <v>5</v>
+      </c>
+      <c r="F5" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="51">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I5" s="48"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A6" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="51">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D6" s="48">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="F6" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="51">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I6" s="48"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A7" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="51">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="D7" s="48">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="F7" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="51">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="I7" s="48"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A8" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="51">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="D8" s="48">
+        <f t="shared" si="2"/>
+        <v>820</v>
+      </c>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="48"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A9" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="51">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="D9" s="48">
+        <f t="shared" si="2"/>
+        <v>85</v>
+      </c>
+      <c r="F9" s="51" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="51" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" s="51">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="I9" s="48"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A10" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="51">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D10" s="48">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="F10" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" s="51">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I10" s="48"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A11" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="51">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="D11" s="48">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="F11" s="51" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" s="51">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="I11" s="48"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A12" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="51">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D12" s="48">
+        <f t="shared" si="2"/>
+        <v>128</v>
+      </c>
+      <c r="F12" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" s="51">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="I12" s="48"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A13" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D13" s="48">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="F13" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="H13" s="51">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="48"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A14" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="48" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="51">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D14" s="48">
+        <f t="shared" si="2"/>
+        <v>142</v>
+      </c>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="51"/>
+      <c r="I14" s="48"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A15" s="48" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="51">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D15" s="48">
+        <f t="shared" si="2"/>
+        <v>243</v>
+      </c>
+      <c r="F15" s="50"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="48"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A16" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="51">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D16" s="48">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="F16" s="50"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="48"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="51">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="D17" s="48">
+        <f t="shared" si="2"/>
+        <v>3373</v>
+      </c>
+      <c r="F17" s="50"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="48"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="51">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="D18" s="48">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="F18" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="G18" s="50">
+        <v>3511</v>
+      </c>
+      <c r="H18" s="57">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="I18" s="48"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="51">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="D19" s="48">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="F19" s="51" t="s">
+        <v>66</v>
+      </c>
+      <c r="G19" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="H19" s="51">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="I19" s="48"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D20" s="48">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="F20" s="50"/>
+      <c r="G20" s="50"/>
+      <c r="H20" s="51">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="48"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="51">
+        <f t="shared" si="0"/>
+        <v>91</v>
+      </c>
+      <c r="D21" s="48">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="F21" s="56">
+        <v>3595</v>
+      </c>
+      <c r="G21" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="H21" s="57">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="I21" s="48"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added MAME code sections, removed all the data section hacks
</commit_message>
<xml_diff>
--- a/memory_map.xlsx
+++ b/memory_map.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="72" windowWidth="29988" windowHeight="13800"/>
+    <workbookView xWindow="384" yWindow="72" windowWidth="29988" windowHeight="13800" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="JETPAC VIC-20 8K+ Expansion" sheetId="6" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="145">
   <si>
     <t>A</t>
   </si>
@@ -146,6 +146,9 @@
     <t>201d</t>
   </si>
   <si>
+    <t>20ac</t>
+  </si>
+  <si>
     <t>20b2</t>
   </si>
   <si>
@@ -173,9 +176,6 @@
     <t>20e2</t>
   </si>
   <si>
-    <t>2416</t>
-  </si>
-  <si>
     <t>244f</t>
   </si>
   <si>
@@ -273,13 +273,211 @@
   </si>
   <si>
     <t>34cc</t>
+  </si>
+  <si>
+    <t>20f2</t>
+  </si>
+  <si>
+    <t>20f7</t>
+  </si>
+  <si>
+    <t>216a</t>
+  </si>
+  <si>
+    <t>2204</t>
+  </si>
+  <si>
+    <t>22e8</t>
+  </si>
+  <si>
+    <t>22ed</t>
+  </si>
+  <si>
+    <t>22f7</t>
+  </si>
+  <si>
+    <t>22ff</t>
+  </si>
+  <si>
+    <t>2313</t>
+  </si>
+  <si>
+    <t>233a</t>
+  </si>
+  <si>
+    <t>235b</t>
+  </si>
+  <si>
+    <t>2375</t>
+  </si>
+  <si>
+    <t>237a</t>
+  </si>
+  <si>
+    <t>2384</t>
+  </si>
+  <si>
+    <t>238c</t>
+  </si>
+  <si>
+    <t>2398</t>
+  </si>
+  <si>
+    <t>239d</t>
+  </si>
+  <si>
+    <t>23c6</t>
+  </si>
+  <si>
+    <t>23d6</t>
+  </si>
+  <si>
+    <t>23f1</t>
+  </si>
+  <si>
+    <t>23f4</t>
+  </si>
+  <si>
+    <t>268b</t>
+  </si>
+  <si>
+    <t>26b3</t>
+  </si>
+  <si>
+    <t>26c4</t>
+  </si>
+  <si>
+    <t>26cd</t>
+  </si>
+  <si>
+    <t>276e</t>
+  </si>
+  <si>
+    <t>277a</t>
+  </si>
+  <si>
+    <t>279e</t>
+  </si>
+  <si>
+    <t>2-Player Game</t>
+  </si>
+  <si>
+    <t>27aa</t>
+  </si>
+  <si>
+    <t>29f0</t>
+  </si>
+  <si>
+    <t>2a07</t>
+  </si>
+  <si>
+    <t>2a14</t>
+  </si>
+  <si>
+    <t>2a45</t>
+  </si>
+  <si>
+    <t>2a4a</t>
+  </si>
+  <si>
+    <t>2a51</t>
+  </si>
+  <si>
+    <t>2a6c</t>
+  </si>
+  <si>
+    <t>2a83</t>
+  </si>
+  <si>
+    <t>2aa1</t>
+  </si>
+  <si>
+    <t>2b16</t>
+  </si>
+  <si>
+    <t>2b7e</t>
+  </si>
+  <si>
+    <t>2b8f</t>
+  </si>
+  <si>
+    <t>2bcc</t>
+  </si>
+  <si>
+    <t>2bd8</t>
+  </si>
+  <si>
+    <t>2be7</t>
+  </si>
+  <si>
+    <t>2bfa</t>
+  </si>
+  <si>
+    <t>2cda</t>
+  </si>
+  <si>
+    <t>2ce3</t>
+  </si>
+  <si>
+    <t>2d4b</t>
+  </si>
+  <si>
+    <t>2d5c</t>
+  </si>
+  <si>
+    <t>2dba</t>
+  </si>
+  <si>
+    <t>2dc5</t>
+  </si>
+  <si>
+    <t>2e9c</t>
+  </si>
+  <si>
+    <t>2ffb</t>
+  </si>
+  <si>
+    <t>2E91</t>
+  </si>
+  <si>
+    <t>309f</t>
+  </si>
+  <si>
+    <t>31b5</t>
+  </si>
+  <si>
+    <t>31bf</t>
+  </si>
+  <si>
+    <t>325e</t>
+  </si>
+  <si>
+    <t>33fe</t>
+  </si>
+  <si>
+    <t>346b</t>
+  </si>
+  <si>
+    <t>349c</t>
+  </si>
+  <si>
+    <t>34c4</t>
+  </si>
+  <si>
+    <t>355e</t>
+  </si>
+  <si>
+    <t>385e</t>
+  </si>
+  <si>
+    <t>code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -334,6 +532,14 @@
       <b/>
       <sz val="20"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -534,7 +740,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -697,6 +903,8 @@
     <xf numFmtId="49" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1000,7 +1208,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -2196,21 +2404,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V21"/>
+  <dimension ref="A1:W75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.77734375" style="48" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.88671875" style="48"/>
     <col min="3" max="3" width="8.77734375" style="50" bestFit="1" customWidth="1"/>
-    <col min="4" max="22" width="8.88671875" style="49"/>
+    <col min="4" max="23" width="8.88671875" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="55" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" s="55" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="52" t="s">
         <v>76</v>
       </c>
@@ -2225,7 +2431,9 @@
       <c r="H1" s="54"/>
       <c r="I1" s="54"/>
       <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
+      <c r="K1" s="54" t="s">
+        <v>107</v>
+      </c>
       <c r="L1" s="54"/>
       <c r="M1" s="54"/>
       <c r="N1" s="54"/>
@@ -2237,8 +2445,9 @@
       <c r="T1" s="54"/>
       <c r="U1" s="54"/>
       <c r="V1" s="54"/>
-    </row>
-    <row r="2" spans="1:22" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="W1" s="54"/>
+    </row>
+    <row r="2" spans="1:23" s="55" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="52" t="s">
         <v>72</v>
       </c>
@@ -2269,13 +2478,14 @@
       <c r="T2" s="54"/>
       <c r="U2" s="54"/>
       <c r="V2" s="54"/>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W2" s="54"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="48" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C3" s="51">
         <f>HEX2DEC(B3)-HEX2DEC(A3)</f>
@@ -2285,41 +2495,29 @@
         <v>77</v>
       </c>
       <c r="G3" s="50" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H3" s="57">
         <f>HEX2DEC(G3)-HEX2DEC(F3)</f>
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A4" s="48" t="s">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C4" s="51"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="57"/>
+      <c r="J4" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K4" s="49">
+        <v>2079</v>
+      </c>
+      <c r="L4" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="51">
-        <f t="shared" ref="C4:C21" si="0">HEX2DEC(B4)-HEX2DEC(A4)</f>
-        <v>5</v>
-      </c>
-      <c r="D4" s="48">
-        <f>HEX2DEC(A4)-HEX2DEC(B3)</f>
-        <v>5</v>
-      </c>
-      <c r="F4" s="51" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" s="51">
-        <f t="shared" ref="H4:H21" si="1">HEX2DEC(G4)-HEX2DEC(F4)</f>
-        <v>5</v>
-      </c>
-      <c r="I4" s="48"/>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="48" t="s">
         <v>37</v>
       </c>
@@ -2327,11 +2525,11 @@
         <v>41</v>
       </c>
       <c r="C5" s="51">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C5:C75" si="0">HEX2DEC(B5)-HEX2DEC(A5)</f>
         <v>5</v>
       </c>
       <c r="D5" s="48">
-        <f t="shared" ref="D5:D21" si="2">HEX2DEC(A5)-HEX2DEC(B4)</f>
+        <f>HEX2DEC(A5)-HEX2DEC(B3)</f>
         <v>5</v>
       </c>
       <c r="F5" s="51" t="s">
@@ -2341,12 +2539,21 @@
         <v>41</v>
       </c>
       <c r="H5" s="51">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="H5:H75" si="1">HEX2DEC(G5)-HEX2DEC(F5)</f>
         <v>5</v>
       </c>
       <c r="I5" s="48"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="J5" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K5" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" s="48" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="48" t="s">
         <v>38</v>
       </c>
@@ -2358,7 +2565,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="48">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="D6:D8" si="2">HEX2DEC(A6)-HEX2DEC(B5)</f>
         <v>5</v>
       </c>
       <c r="F6" s="51" t="s">
@@ -2372,372 +2579,1292 @@
         <v>5</v>
       </c>
       <c r="I6" s="48"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="J6" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K6" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" s="51" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="48" t="s">
-        <v>44</v>
-      </c>
       <c r="C7" s="51">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D7" s="48">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="F7" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="51" t="s">
         <v>43</v>
-      </c>
-      <c r="G7" s="51" t="s">
-        <v>44</v>
       </c>
       <c r="H7" s="51">
         <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I7" s="48"/>
+      <c r="J7" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K7" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="L7" s="51" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A8" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="51">
+        <f t="shared" si="0"/>
         <v>18</v>
-      </c>
-      <c r="I7" s="48"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A8" s="48" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="51">
-        <f t="shared" si="0"/>
-        <v>57</v>
       </c>
       <c r="D8" s="48">
         <f t="shared" si="2"/>
-        <v>820</v>
-      </c>
-      <c r="F8" s="50"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="51"/>
+        <v>5</v>
+      </c>
+      <c r="F8" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="51" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="51">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
       <c r="I8" s="48"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A9" s="48" t="s">
+      <c r="J8" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K8" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="L8" s="51" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C9" s="51"/>
+      <c r="D9" s="48"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K9" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="L9" s="51" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C10" s="51"/>
+      <c r="D10" s="48"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K10" s="49">
+        <v>2173</v>
+      </c>
+      <c r="L10" s="51" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C11" s="51"/>
+      <c r="D11" s="48"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K11" s="49">
+        <v>2211</v>
+      </c>
+      <c r="L11" s="51" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C12" s="51"/>
+      <c r="D12" s="48"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K12" s="49" t="s">
+        <v>84</v>
+      </c>
+      <c r="L12" s="51" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C13" s="51"/>
+      <c r="D13" s="48"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K13" s="49" t="s">
+        <v>86</v>
+      </c>
+      <c r="L13" s="51" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C14" s="51"/>
+      <c r="D14" s="48"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="51"/>
+      <c r="I14" s="48"/>
+      <c r="J14" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K14" s="49">
+        <v>2318</v>
+      </c>
+      <c r="L14" s="51" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C15" s="51"/>
+      <c r="D15" s="48"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="48"/>
+      <c r="J15" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K15" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="L15" s="51" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C16" s="51"/>
+      <c r="D16" s="48"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="51"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="48"/>
+      <c r="J16" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K16" s="49" t="s">
+        <v>91</v>
+      </c>
+      <c r="L16" s="51" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C17" s="51"/>
+      <c r="D17" s="48"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K17" s="49" t="s">
+        <v>93</v>
+      </c>
+      <c r="L17" s="51" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C18" s="51"/>
+      <c r="D18" s="48"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K18" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="L18" s="51" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C19" s="51"/>
+      <c r="D19" s="48"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K19" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="L19" s="51" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C20" s="51"/>
+      <c r="D20" s="48"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="48"/>
+      <c r="J20" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K20" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="L20" s="51" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="48" t="s">
+      <c r="B21" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="51">
+      <c r="C21" s="51">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="D9" s="48">
-        <f t="shared" si="2"/>
-        <v>85</v>
-      </c>
-      <c r="F9" s="51" t="s">
+      <c r="D21" s="48"/>
+      <c r="F21" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="51" t="s">
+      <c r="G21" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="H9" s="51">
+      <c r="H21" s="51">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="I9" s="48"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A10" s="48" t="s">
+      <c r="I21" s="48"/>
+      <c r="J21" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K21" s="49" t="s">
+        <v>47</v>
+      </c>
+      <c r="L21" s="51" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="B22" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="51">
+      <c r="C22" s="51">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D10" s="48">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-      <c r="F10" s="51" t="s">
+      <c r="D22" s="48"/>
+      <c r="F22" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="G10" s="51" t="s">
+      <c r="G22" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="H10" s="51">
+      <c r="H22" s="51">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="I10" s="48"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A11" s="48" t="s">
+      <c r="I22" s="48"/>
+      <c r="J22" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K22" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="L22" s="51" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="48" t="s">
+      <c r="B23" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="51">
+      <c r="C23" s="51">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="D11" s="48">
-        <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="F11" s="51" t="s">
+      <c r="D23" s="48"/>
+      <c r="F23" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="51" t="s">
+      <c r="G23" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="H11" s="51">
+      <c r="H23" s="51">
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="I11" s="48"/>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A12" s="48" t="s">
+      <c r="I23" s="48"/>
+      <c r="J23" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K23" s="51" t="s">
+        <v>51</v>
+      </c>
+      <c r="L23" s="51" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="48" t="s">
+      <c r="B24" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="51">
+      <c r="C24" s="51">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="D12" s="48">
-        <f t="shared" si="2"/>
-        <v>128</v>
-      </c>
-      <c r="F12" s="51" t="s">
+      <c r="D24" s="48"/>
+      <c r="F24" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="G12" s="51" t="s">
+      <c r="G24" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="H12" s="51">
+      <c r="H24" s="51">
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="I12" s="48"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A13" s="48" t="s">
+      <c r="I24" s="48"/>
+      <c r="J24" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K24" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="L24" s="49">
+        <v>2676</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="48" t="s">
+      <c r="B25" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="51">
+      <c r="C25" s="51">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D13" s="48">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="F13" s="51" t="s">
+      <c r="D25" s="48"/>
+      <c r="F25" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="G13" s="51" t="s">
+      <c r="G25" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="H13" s="51">
+      <c r="H25" s="51">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I13" s="48"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A14" s="48" t="s">
+      <c r="I25" s="48"/>
+      <c r="J25" s="49" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="48" t="s">
+      <c r="B26" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="51">
+      <c r="C26" s="51">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="D14" s="48">
-        <f t="shared" si="2"/>
+      <c r="D26" s="48"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="50"/>
+      <c r="H26" s="51"/>
+      <c r="I26" s="48"/>
+      <c r="J26" s="49" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C27" s="51"/>
+      <c r="D27" s="48"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="50"/>
+      <c r="H27" s="51"/>
+      <c r="I27" s="48"/>
+      <c r="J27" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K27" s="49">
+        <v>2682</v>
+      </c>
+      <c r="L27" s="49" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C28" s="51"/>
+      <c r="D28" s="48"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="51"/>
+      <c r="I28" s="48"/>
+      <c r="J28" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K28" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="L28" s="49" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C29" s="51"/>
+      <c r="D29" s="48"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="51"/>
+      <c r="I29" s="48"/>
+      <c r="J29" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K29" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="L29" s="49">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C30" s="51"/>
+      <c r="D30" s="48"/>
+      <c r="F30" s="50"/>
+      <c r="G30" s="50"/>
+      <c r="H30" s="51"/>
+      <c r="I30" s="48"/>
+      <c r="J30" s="49" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C31" s="51"/>
+      <c r="D31" s="48"/>
+      <c r="F31" s="50"/>
+      <c r="G31" s="50"/>
+      <c r="H31" s="51"/>
+      <c r="I31" s="48"/>
+      <c r="J31" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K31" s="49">
+        <v>2755</v>
+      </c>
+      <c r="L31" s="49" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C32" s="51"/>
+      <c r="D32" s="48"/>
+      <c r="F32" s="50"/>
+      <c r="G32" s="50"/>
+      <c r="H32" s="51"/>
+      <c r="I32" s="48"/>
+      <c r="J32" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K32" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="L32" s="49" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C33" s="51"/>
+      <c r="D33" s="48"/>
+      <c r="F33" s="50"/>
+      <c r="G33" s="50"/>
+      <c r="H33" s="51"/>
+      <c r="I33" s="48"/>
+      <c r="J33" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K33" s="49">
+        <v>2790</v>
+      </c>
+      <c r="L33" s="49" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="34" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C34" s="51"/>
+      <c r="D34" s="48"/>
+      <c r="F34" s="50"/>
+      <c r="G34" s="50"/>
+      <c r="H34" s="51"/>
+      <c r="I34" s="48"/>
+      <c r="J34" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K34" s="49" t="s">
+        <v>108</v>
+      </c>
+      <c r="L34" s="49">
+        <v>2839</v>
+      </c>
+    </row>
+    <row r="35" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C35" s="51"/>
+      <c r="D35" s="48"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="50"/>
+      <c r="H35" s="51"/>
+      <c r="I35" s="48"/>
+      <c r="J35" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K35" s="49">
+        <v>2844</v>
+      </c>
+      <c r="L35" s="49">
+        <v>2869</v>
+      </c>
+    </row>
+    <row r="36" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C36" s="51"/>
+      <c r="D36" s="48"/>
+      <c r="F36" s="50"/>
+      <c r="G36" s="50"/>
+      <c r="H36" s="51"/>
+      <c r="I36" s="48"/>
+      <c r="J36" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K36" s="49">
+        <v>2874</v>
+      </c>
+      <c r="L36" s="49">
+        <v>2887</v>
+      </c>
+    </row>
+    <row r="37" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C37" s="51"/>
+      <c r="D37" s="48"/>
+      <c r="F37" s="50"/>
+      <c r="G37" s="50"/>
+      <c r="H37" s="51"/>
+      <c r="I37" s="48"/>
+      <c r="J37" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K37" s="49">
+        <v>2892</v>
+      </c>
+      <c r="L37" s="49">
+        <v>2966</v>
+      </c>
+    </row>
+    <row r="38" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C38" s="51"/>
+      <c r="D38" s="48"/>
+      <c r="F38" s="50"/>
+      <c r="G38" s="50"/>
+      <c r="H38" s="51"/>
+      <c r="I38" s="48"/>
+      <c r="J38" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K38" s="49">
+        <v>2977</v>
+      </c>
+      <c r="L38" s="49">
+        <v>2990</v>
+      </c>
+    </row>
+    <row r="39" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C39" s="51"/>
+      <c r="D39" s="48"/>
+      <c r="F39" s="50"/>
+      <c r="G39" s="50"/>
+      <c r="H39" s="51"/>
+      <c r="I39" s="48"/>
+      <c r="J39" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K39" s="49">
+        <v>2997</v>
+      </c>
+      <c r="L39" s="49" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="40" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C40" s="51"/>
+      <c r="D40" s="48"/>
+      <c r="F40" s="50"/>
+      <c r="G40" s="50"/>
+      <c r="H40" s="51"/>
+      <c r="I40" s="48"/>
+      <c r="J40" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K40" s="49" t="s">
+        <v>110</v>
+      </c>
+      <c r="L40" s="49" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="41" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C41" s="51"/>
+      <c r="D41" s="48"/>
+      <c r="F41" s="50"/>
+      <c r="G41" s="50"/>
+      <c r="H41" s="51"/>
+      <c r="I41" s="48"/>
+      <c r="J41" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K41" s="49" t="s">
+        <v>112</v>
+      </c>
+      <c r="L41" s="49" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="42" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C42" s="51"/>
+      <c r="D42" s="48"/>
+      <c r="F42" s="50"/>
+      <c r="G42" s="50"/>
+      <c r="H42" s="51"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K42" s="58" t="s">
+        <v>114</v>
+      </c>
+      <c r="L42" s="59" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="43" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C43" s="51"/>
+      <c r="D43" s="48"/>
+      <c r="F43" s="50"/>
+      <c r="G43" s="50"/>
+      <c r="H43" s="51"/>
+      <c r="I43" s="48"/>
+      <c r="J43" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K43" s="49" t="s">
+        <v>116</v>
+      </c>
+      <c r="L43" s="59" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="44" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C44" s="51"/>
+      <c r="D44" s="48"/>
+      <c r="F44" s="50"/>
+      <c r="G44" s="50"/>
+      <c r="H44" s="51"/>
+      <c r="I44" s="48"/>
+      <c r="J44" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K44" s="49" t="s">
+        <v>118</v>
+      </c>
+      <c r="L44" s="59" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="45" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C45" s="51"/>
+      <c r="D45" s="48"/>
+      <c r="F45" s="50"/>
+      <c r="G45" s="50"/>
+      <c r="H45" s="51"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K45" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="L45" s="59" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="46" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C46" s="51"/>
+      <c r="D46" s="48"/>
+      <c r="F46" s="50"/>
+      <c r="G46" s="50"/>
+      <c r="H46" s="51"/>
+      <c r="I46" s="48"/>
+      <c r="J46" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K46" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="L46" s="59" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="47" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C47" s="51"/>
+      <c r="D47" s="48"/>
+      <c r="F47" s="50"/>
+      <c r="G47" s="50"/>
+      <c r="H47" s="51"/>
+      <c r="I47" s="48"/>
+      <c r="J47" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K47" s="49" t="s">
+        <v>124</v>
+      </c>
+      <c r="L47" s="59" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="48" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C48" s="51"/>
+      <c r="D48" s="48"/>
+      <c r="F48" s="50"/>
+      <c r="G48" s="50"/>
+      <c r="H48" s="51"/>
+      <c r="I48" s="48"/>
+      <c r="J48" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K48" s="49" t="s">
+        <v>126</v>
+      </c>
+      <c r="L48" s="59" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="49" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C49" s="51"/>
+      <c r="D49" s="48"/>
+      <c r="F49" s="50"/>
+      <c r="G49" s="50"/>
+      <c r="H49" s="51"/>
+      <c r="I49" s="48"/>
+      <c r="J49" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K49" s="49" t="s">
+        <v>128</v>
+      </c>
+      <c r="L49" s="59" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="50" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C50" s="51"/>
+      <c r="D50" s="48"/>
+      <c r="F50" s="50"/>
+      <c r="G50" s="50"/>
+      <c r="H50" s="51"/>
+      <c r="I50" s="48"/>
+      <c r="J50" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K50" s="49" t="s">
+        <v>130</v>
+      </c>
+      <c r="L50" s="48" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="51" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C51" s="51"/>
+      <c r="D51" s="48"/>
+      <c r="F51" s="50"/>
+      <c r="G51" s="50"/>
+      <c r="H51" s="51"/>
+      <c r="I51" s="48"/>
+      <c r="J51" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K51" s="49" t="s">
+        <v>131</v>
+      </c>
+      <c r="L51" s="59" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="52" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C52" s="51"/>
+      <c r="D52" s="48"/>
+      <c r="F52" s="50"/>
+      <c r="G52" s="50"/>
+      <c r="H52" s="51"/>
+      <c r="I52" s="48"/>
+      <c r="J52" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K52" s="49">
+        <v>3000</v>
+      </c>
+      <c r="L52" s="49">
+        <v>3069</v>
+      </c>
+    </row>
+    <row r="53" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C53" s="51"/>
+      <c r="D53" s="48"/>
+      <c r="F53" s="50"/>
+      <c r="G53" s="50"/>
+      <c r="H53" s="51"/>
+      <c r="I53" s="48"/>
+      <c r="J53" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K53" s="49">
+        <v>3070</v>
+      </c>
+      <c r="L53" s="49">
+        <v>3093</v>
+      </c>
+    </row>
+    <row r="54" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C54" s="51"/>
+      <c r="D54" s="48"/>
+      <c r="F54" s="50"/>
+      <c r="G54" s="50"/>
+      <c r="H54" s="51"/>
+      <c r="I54" s="48"/>
+      <c r="J54" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K54" s="49" t="s">
+        <v>134</v>
+      </c>
+      <c r="L54" s="49" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="55" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C55" s="51"/>
+      <c r="D55" s="48"/>
+      <c r="F55" s="50"/>
+      <c r="G55" s="50"/>
+      <c r="H55" s="51"/>
+      <c r="I55" s="48"/>
+      <c r="J55" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K55" s="49" t="s">
+        <v>136</v>
+      </c>
+      <c r="L55" s="49">
+        <v>3253</v>
+      </c>
+    </row>
+    <row r="56" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C56" s="51"/>
+      <c r="D56" s="48"/>
+      <c r="F56" s="50"/>
+      <c r="G56" s="50"/>
+      <c r="H56" s="51"/>
+      <c r="I56" s="48"/>
+      <c r="J56" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K56" s="49" t="s">
+        <v>137</v>
+      </c>
+      <c r="L56" s="49" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="57" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C57" s="51"/>
+      <c r="D57" s="48"/>
+      <c r="F57" s="50"/>
+      <c r="G57" s="50"/>
+      <c r="H57" s="51"/>
+      <c r="I57" s="48"/>
+      <c r="J57" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K57" s="49">
+        <v>3465</v>
+      </c>
+      <c r="L57" s="49" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="58" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C58" s="51"/>
+      <c r="D58" s="48"/>
+      <c r="F58" s="50"/>
+      <c r="G58" s="50"/>
+      <c r="H58" s="51"/>
+      <c r="I58" s="48"/>
+      <c r="J58" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K58" s="49">
+        <v>3475</v>
+      </c>
+      <c r="L58" s="49" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="59" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C59" s="51"/>
+      <c r="D59" s="48"/>
+      <c r="F59" s="50"/>
+      <c r="G59" s="50"/>
+      <c r="H59" s="51"/>
+      <c r="I59" s="48"/>
+      <c r="J59" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K59" s="49" t="s">
+        <v>62</v>
+      </c>
+      <c r="L59" s="49" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="60" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C60" s="51"/>
+      <c r="D60" s="48"/>
+      <c r="F60" s="50"/>
+      <c r="G60" s="50"/>
+      <c r="H60" s="51"/>
+      <c r="I60" s="48"/>
+      <c r="J60" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K60" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="L60" s="49">
+        <v>3511</v>
+      </c>
+    </row>
+    <row r="61" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C61" s="51"/>
+      <c r="D61" s="48"/>
+      <c r="F61" s="50"/>
+      <c r="G61" s="50"/>
+      <c r="H61" s="51"/>
+      <c r="I61" s="48"/>
+      <c r="J61" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K61" s="49">
+        <v>3520</v>
+      </c>
+      <c r="L61" s="59">
+        <v>3544</v>
+      </c>
+    </row>
+    <row r="62" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C62" s="51"/>
+      <c r="D62" s="48"/>
+      <c r="F62" s="50"/>
+      <c r="G62" s="50"/>
+      <c r="H62" s="51"/>
+      <c r="I62" s="48"/>
+      <c r="J62" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K62" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="L62" s="59" t="s">
         <v>142</v>
       </c>
-      <c r="F14" s="50"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="51"/>
-      <c r="I14" s="48"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A15" s="48" t="s">
+    </row>
+    <row r="63" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C63" s="51"/>
+      <c r="D63" s="48"/>
+      <c r="F63" s="50"/>
+      <c r="G63" s="50"/>
+      <c r="H63" s="51"/>
+      <c r="I63" s="48"/>
+      <c r="J63" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K63" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="L63" s="59" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="64" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C64" s="51"/>
+      <c r="D64" s="48"/>
+      <c r="F64" s="50"/>
+      <c r="G64" s="50"/>
+      <c r="H64" s="51"/>
+      <c r="I64" s="48"/>
+      <c r="J64" s="48"/>
+      <c r="L64" s="59"/>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C65" s="51"/>
+      <c r="D65" s="48"/>
+      <c r="F65" s="50"/>
+      <c r="G65" s="50"/>
+      <c r="H65" s="51"/>
+      <c r="I65" s="48"/>
+      <c r="J65" s="48"/>
+      <c r="L65" s="59"/>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C66" s="51"/>
+      <c r="D66" s="48"/>
+      <c r="F66" s="50"/>
+      <c r="G66" s="50"/>
+      <c r="H66" s="51"/>
+      <c r="I66" s="48"/>
+      <c r="J66" s="48"/>
+      <c r="L66" s="59"/>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C67" s="51"/>
+      <c r="D67" s="48"/>
+      <c r="F67" s="50"/>
+      <c r="G67" s="50"/>
+      <c r="H67" s="51"/>
+      <c r="I67" s="48"/>
+      <c r="J67" s="48"/>
+      <c r="L67" s="59"/>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C68" s="51"/>
+      <c r="D68" s="48"/>
+      <c r="F68" s="50"/>
+      <c r="G68" s="50"/>
+      <c r="H68" s="51"/>
+      <c r="I68" s="48"/>
+      <c r="J68" s="48"/>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A69" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="48" t="s">
+      <c r="B69" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="51">
+      <c r="C69" s="51">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="D15" s="48">
-        <f t="shared" si="2"/>
-        <v>243</v>
-      </c>
-      <c r="F15" s="50"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="51"/>
-      <c r="I15" s="48"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A16" s="48" t="s">
+      <c r="D69" s="48"/>
+      <c r="F69" s="50"/>
+      <c r="G69" s="50"/>
+      <c r="H69" s="51"/>
+      <c r="I69" s="48"/>
+      <c r="J69" s="48"/>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A70" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="48" t="s">
+      <c r="B70" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="51">
+      <c r="C70" s="51">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="D16" s="48">
-        <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-      <c r="F16" s="50"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="51"/>
-      <c r="I16" s="48"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="48" t="s">
+      <c r="D70" s="48"/>
+      <c r="F70" s="50"/>
+      <c r="G70" s="50"/>
+      <c r="H70" s="51"/>
+      <c r="I70" s="48"/>
+      <c r="J70" s="48"/>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A71" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="48" t="s">
+      <c r="B71" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="51">
+      <c r="C71" s="51">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="D17" s="48">
-        <f t="shared" si="2"/>
-        <v>3373</v>
-      </c>
-      <c r="F17" s="50"/>
-      <c r="G17" s="50"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="48"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="48" t="s">
+      <c r="D71" s="48"/>
+      <c r="F71" s="50"/>
+      <c r="G71" s="50"/>
+      <c r="H71" s="51"/>
+      <c r="I71" s="48"/>
+      <c r="J71" s="48"/>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A72" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="48" t="s">
+      <c r="B72" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="51">
+      <c r="C72" s="51">
         <f t="shared" si="0"/>
         <v>74</v>
       </c>
-      <c r="D18" s="48">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="F18" s="56" t="s">
+      <c r="D72" s="48"/>
+      <c r="F72" s="56" t="s">
         <v>78</v>
       </c>
-      <c r="G18" s="50">
+      <c r="G72" s="50">
         <v>3511</v>
       </c>
-      <c r="H18" s="57">
+      <c r="H72" s="57">
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
-      <c r="I18" s="48"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="48" t="s">
+      <c r="I72" s="48"/>
+      <c r="J72" s="48"/>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A73" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="B19" s="48" t="s">
+      <c r="B73" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="51">
+      <c r="C73" s="51">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="D19" s="48">
-        <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="F19" s="51" t="s">
+      <c r="D73" s="48"/>
+      <c r="F73" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="G19" s="51" t="s">
+      <c r="G73" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="H19" s="51">
+      <c r="H73" s="51">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="I19" s="48"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="48" t="s">
+      <c r="I73" s="48"/>
+      <c r="J73" s="48"/>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A74" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="B20" s="48" t="s">
+      <c r="B74" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="C20" s="51">
+      <c r="C74" s="51">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D20" s="48">
-        <f t="shared" si="2"/>
-        <v>24</v>
-      </c>
-      <c r="F20" s="50"/>
-      <c r="G20" s="50"/>
-      <c r="H20" s="51">
+      <c r="D74" s="48"/>
+      <c r="F74" s="50"/>
+      <c r="G74" s="50"/>
+      <c r="H74" s="51">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I20" s="48"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="48" t="s">
+      <c r="I74" s="48"/>
+      <c r="J74" s="48"/>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A75" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="B21" s="48" t="s">
+      <c r="B75" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="C21" s="51">
+      <c r="C75" s="51">
         <f t="shared" si="0"/>
         <v>91</v>
       </c>
-      <c r="D21" s="48">
-        <f t="shared" si="2"/>
-        <v>31</v>
-      </c>
-      <c r="F21" s="56">
+      <c r="D75" s="48"/>
+      <c r="F75" s="56">
         <v>3595</v>
       </c>
-      <c r="G21" s="51" t="s">
+      <c r="G75" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="H21" s="57">
+      <c r="H75" s="57">
         <f t="shared" si="1"/>
         <v>65</v>
       </c>
-      <c r="I21" s="48"/>
+      <c r="I75" s="48"/>
+      <c r="J75" s="48"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>